<commit_message>
moved r_script files around
</commit_message>
<xml_diff>
--- a/scripts/r_scripts/heatmaps_clusters.xlsx
+++ b/scripts/r_scripts/heatmaps_clusters.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/Desktop/software/tax-e/scripts/r_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7B448651-1344-DD4A-88D4-C4D3D0E9779D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C236C961-0342-1140-BAF2-2C6D8C5492E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Log_norm" sheetId="1" r:id="rId1"/>
-    <sheet name="TF_norm" sheetId="2" r:id="rId2"/>
-    <sheet name="Trans_assoc_GO_terms" sheetId="6" r:id="rId3"/>
-    <sheet name="Test Data" sheetId="7" r:id="rId4"/>
-    <sheet name="Neg_log_TF_norm" sheetId="3" r:id="rId5"/>
-    <sheet name="Aug_freq_norm" sheetId="4" r:id="rId6"/>
-    <sheet name="ATPase_activity" sheetId="5" r:id="rId7"/>
+    <sheet name="Log_norm_d1" sheetId="1" r:id="rId1"/>
+    <sheet name="Log_norm_d2" sheetId="8" r:id="rId2"/>
+    <sheet name="TF_norm_d1" sheetId="2" r:id="rId3"/>
+    <sheet name="Trans_assoc_GO_terms_d1" sheetId="6" r:id="rId4"/>
+    <sheet name="Test Data_d1" sheetId="7" r:id="rId5"/>
+    <sheet name="Neg_log_TF_norm_d1" sheetId="3" r:id="rId6"/>
+    <sheet name="Aug_freq_norm_d1" sheetId="4" r:id="rId7"/>
+    <sheet name="ATPase_activity_d1" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Log_norm!$G$7:$G$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Log_norm_d1!$G$7:$G$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="472" uniqueCount="261">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="577" uniqueCount="276">
   <si>
     <t>GO:0019281</t>
   </si>
@@ -817,6 +818,51 @@
   </si>
   <si>
     <t>freshwater ontario lake</t>
+  </si>
+  <si>
+    <t>GO:0006183</t>
+  </si>
+  <si>
+    <t>GO:0006228</t>
+  </si>
+  <si>
+    <t>GO:0006222</t>
+  </si>
+  <si>
+    <t>GO:0015991</t>
+  </si>
+  <si>
+    <t>GO Cluster</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0015991</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0006222</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0006228</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0006183</t>
+  </si>
+  <si>
+    <t>ATP hydrolysis coupled proton transport</t>
+  </si>
+  <si>
+    <t>UMP biosynthetic process</t>
+  </si>
+  <si>
+    <t>UTP biosynthetic process</t>
+  </si>
+  <si>
+    <t>GTP biosynthetic process</t>
+  </si>
+  <si>
+    <t>nucleoside biosynthetic process</t>
+  </si>
+  <si>
+    <t>proton transmembrane transport</t>
   </si>
 </sst>
 </file>
@@ -1686,8 +1732,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2275,6 +2321,498 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6302A608-DD57-D34E-B2B7-62049E68FABE}">
+  <dimension ref="B6:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="50.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C27" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>273</v>
+      </c>
+      <c r="F27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>156</v>
+      </c>
+      <c r="F30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B7:C31">
+    <sortCondition descending="1" ref="B7:B31"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{267DF03A-CBCB-F24A-9B67-04248C38ED3D}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{F5A93F2C-1888-334C-84D9-35E98662EF73}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{D03E49CA-D14A-4E43-9026-64BD60C783FD}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{8D3C7613-5B58-A148-A023-1235DDFFD2A9}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{946D069D-7EC5-0A46-9595-9DA8EF713EF7}"/>
+    <hyperlink ref="B12" r:id="rId6" xr:uid="{7523B634-C8B3-5647-B7C4-CF6D3F7BF0A1}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{91BE3F06-C445-4C4A-B142-2A88F63D5AD0}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{04781286-505A-434D-83E6-ADE654E6EADF}"/>
+    <hyperlink ref="B15" r:id="rId9" xr:uid="{396799F4-AA62-6943-AEB2-CA37F141C433}"/>
+    <hyperlink ref="B16" r:id="rId10" xr:uid="{1E14A84A-593D-D947-A097-76931EE2869B}"/>
+    <hyperlink ref="B17" r:id="rId11" xr:uid="{FBB3CB9B-C886-7D4D-A655-EC978ABD20C1}"/>
+    <hyperlink ref="B18" r:id="rId12" xr:uid="{307BB20C-7C76-CF4F-9F71-38954D59CF0B}"/>
+    <hyperlink ref="B19" r:id="rId13" xr:uid="{55AE6087-6A41-5048-BC44-84B03BFF33A1}"/>
+    <hyperlink ref="B20" r:id="rId14" xr:uid="{29B96C57-8655-0140-85AE-B309836E6F2C}"/>
+    <hyperlink ref="B21" r:id="rId15" xr:uid="{5837222F-E658-7149-A1AC-6B83DE163F9F}"/>
+    <hyperlink ref="B22" r:id="rId16" xr:uid="{2DCCD717-1E4C-AE43-BB8F-7643EB8E6E05}"/>
+    <hyperlink ref="B23" r:id="rId17" xr:uid="{74A81809-8950-904A-8BE6-3CDF8C53AB34}"/>
+    <hyperlink ref="B24" r:id="rId18" xr:uid="{36AD2E73-B84C-DA4F-9793-BFB868284342}"/>
+    <hyperlink ref="B25" r:id="rId19" xr:uid="{75C26458-D1B1-F946-8106-0776462AFC75}"/>
+    <hyperlink ref="B26" r:id="rId20" xr:uid="{B23B4484-F7F7-7B4D-8F52-CBBD62D21D15}"/>
+    <hyperlink ref="B27" r:id="rId21" xr:uid="{4C90CAB8-C441-4149-97C3-73B108A21A31}"/>
+    <hyperlink ref="B28" r:id="rId22" xr:uid="{089E76C0-86CD-6D4C-A71B-9EC923448C1D}"/>
+    <hyperlink ref="B29" r:id="rId23" xr:uid="{9B4CE07D-DE01-4A45-9CBA-1960D2C76269}"/>
+    <hyperlink ref="B30" r:id="rId24" xr:uid="{C7B6B6F9-25ED-7F40-82F5-73484D7200F0}"/>
+    <hyperlink ref="B31" r:id="rId25" xr:uid="{16DF9BD6-472E-A14F-A907-702A541684E5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -2865,7 +3403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97824A00-ECFF-7A42-8C3C-22BE9B58A94E}">
   <dimension ref="B1:C13"/>
   <sheetViews>
@@ -2985,11 +3523,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8CCC5F-0E7D-8B4B-9B29-0808A70AE5F7}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -3041,11 +3579,11 @@
         <v>2097</v>
       </c>
       <c r="H2">
-        <f>E2/D2*100</f>
+        <f t="shared" ref="H2:H7" si="0">E2/D2*100</f>
         <v>55.099894847528915</v>
       </c>
       <c r="I2">
-        <f>F2/D2*100</f>
+        <f t="shared" ref="I2:I7" si="1">F2/D2*100</f>
         <v>55.126182965299684</v>
       </c>
     </row>
@@ -3069,11 +3607,11 @@
         <v>70012</v>
       </c>
       <c r="H3">
-        <f>E3/D3*100</f>
+        <f t="shared" si="0"/>
         <v>47.001437825636586</v>
       </c>
       <c r="I3">
-        <f>F3/D3*100</f>
+        <f t="shared" si="1"/>
         <v>54.120993800343221</v>
       </c>
     </row>
@@ -3097,11 +3635,11 @@
         <v>1693</v>
       </c>
       <c r="H4">
-        <f>E4/D4*100</f>
+        <f t="shared" si="0"/>
         <v>52.757868494858208</v>
       </c>
       <c r="I4">
-        <f>F4/D4*100</f>
+        <f t="shared" si="1"/>
         <v>52.757868494858208</v>
       </c>
     </row>
@@ -3125,11 +3663,11 @@
         <v>223192</v>
       </c>
       <c r="H5">
-        <f>E5/D5*100</f>
+        <f t="shared" si="0"/>
         <v>39.402056712291085</v>
       </c>
       <c r="I5">
-        <f>F5/D5*100</f>
+        <f t="shared" si="1"/>
         <v>52.033748545823741</v>
       </c>
     </row>
@@ -3153,11 +3691,11 @@
         <v>2516573</v>
       </c>
       <c r="H6">
-        <f>E6/D6*100</f>
+        <f t="shared" si="0"/>
         <v>40.006106776288007</v>
       </c>
       <c r="I6">
-        <f>F6/D6*100</f>
+        <f t="shared" si="1"/>
         <v>53.030187451480835</v>
       </c>
     </row>
@@ -3181,11 +3719,11 @@
         <v>126892</v>
       </c>
       <c r="H7">
-        <f>E7/D7*100</f>
+        <f t="shared" si="0"/>
         <v>39.623193869080318</v>
       </c>
       <c r="I7">
-        <f>F7/D7*100</f>
+        <f t="shared" si="1"/>
         <v>50.887274973030848</v>
       </c>
     </row>
@@ -3194,12 +3732,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3429,12 +3967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A4:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3661,7 +4199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30514106-9061-1344-8525-A9B566C1A4CA}">
   <dimension ref="B3:E22"/>
   <sheetViews>

</xml_diff>